<commit_message>
Add updated data files (csv and xlsx)
</commit_message>
<xml_diff>
--- a/data/raw_data/final_project_culturing_counts.xlsx
+++ b/data/raw_data/final_project_culturing_counts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bellafinn/Desktop/Microbiology_Project_SP2019/ifinney-microbiology-project/data/raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F910DD0C-158B-E541-9E8E-601884E86852}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA8B230C-E3A7-2B4A-97B3-A88BA8BD765E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="14660" xr2:uid="{BE2D5990-80EE-CB4A-9738-3FDE4723E557}"/>
+    <workbookView xWindow="140" yWindow="460" windowWidth="25440" windowHeight="14660" xr2:uid="{BE2D5990-80EE-CB4A-9738-3FDE4723E557}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="20">
   <si>
     <t>location_name_or_control</t>
   </si>
@@ -90,9 +90,6 @@
   </si>
   <si>
     <t>california_poppy</t>
-  </si>
-  <si>
-    <t>white_foam</t>
   </si>
 </sst>
 </file>
@@ -463,8 +460,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6C64FA7-60D5-1645-A8A3-6235FCA6E8D3}">
   <dimension ref="A1:K108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="C113" sqref="C113"/>
+    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="A107" sqref="A107:XFD108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2312,38 +2309,18 @@
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A107" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B107" s="2">
-        <v>3</v>
-      </c>
-      <c r="C107" s="2">
-        <v>1</v>
-      </c>
-      <c r="D107" s="2">
-        <v>1</v>
-      </c>
-      <c r="E107" s="2">
-        <v>1000</v>
-      </c>
+      <c r="A107" s="2"/>
+      <c r="B107" s="2"/>
+      <c r="C107" s="2"/>
+      <c r="D107" s="2"/>
+      <c r="E107" s="2"/>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A108" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B108" s="2">
-        <v>4</v>
-      </c>
-      <c r="C108" s="2">
-        <v>1</v>
-      </c>
-      <c r="D108" s="2">
-        <v>1</v>
-      </c>
-      <c r="E108" s="2">
-        <v>1000</v>
-      </c>
+      <c r="A108" s="2"/>
+      <c r="B108" s="2"/>
+      <c r="C108" s="2"/>
+      <c r="D108" s="2"/>
+      <c r="E108" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>